<commit_message>
added user_objects to kiki.py
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hadi\Desktop\kiki_crypto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6B1BB9-8724-4E47-9E8D-EC30E1B2A985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043DB5F1-3D24-46C0-9075-BAE3545970E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12419" uniqueCount="1185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12417" uniqueCount="1185">
   <si>
     <t>UserNum</t>
   </si>
@@ -4041,7 +4041,7 @@
   <dimension ref="A1:V1129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K1128"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4135,9 +4135,7 @@
       <c r="B2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>1181</v>
-      </c>
+      <c r="C2" s="11"/>
       <c r="D2" s="2">
         <v>1000</v>
       </c>
@@ -4153,9 +4151,7 @@
       <c r="H2" s="4">
         <v>20</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>1183</v>
-      </c>
+      <c r="I2" s="11"/>
       <c r="J2" s="4">
         <v>14000</v>
       </c>

</xml_diff>

<commit_message>
testing with twitter scraping using proxy
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hadi\Desktop\kiki_crypto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CC5EDA-1E20-4C63-AAE5-4739B981D5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1397E06-DD7C-4D3B-AE11-8BF40CCDF1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6888,9 +6888,6 @@
     <t>https://www.instagram.com/pubity/</t>
   </si>
   <si>
-    <t>https://www.instagram.com/laurengerman/</t>
-  </si>
-  <si>
     <t>https://www.instagram.com/officialtomellis/</t>
   </si>
   <si>
@@ -6949,6 +6946,9 @@
   </si>
   <si>
     <t>Maha</t>
+  </si>
+  <si>
+    <t>https://x.com/ordinalHO?t=jkhlbh&amp;s=04</t>
   </si>
 </sst>
 </file>
@@ -7423,7 +7423,7 @@
   <dimension ref="A1:V1129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7515,10 +7515,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>2287</v>
+        <v>2307</v>
       </c>
       <c r="D2" s="2">
         <v>1000</v>
@@ -7583,7 +7583,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>2286</v>
@@ -7651,10 +7651,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>2288</v>
+        <v>2287</v>
       </c>
       <c r="D4" s="2">
         <v>3000</v>
@@ -7719,10 +7719,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>2299</v>
+        <v>2298</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>2289</v>
+        <v>2288</v>
       </c>
       <c r="D5" s="2">
         <v>4000</v>
@@ -7787,10 +7787,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
       <c r="D6" s="2">
         <v>5000</v>
@@ -7855,10 +7855,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>2301</v>
+        <v>2300</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
       <c r="D7" s="2">
         <v>6000</v>
@@ -7923,10 +7923,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>2302</v>
+        <v>2301</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>2292</v>
+        <v>2291</v>
       </c>
       <c r="D8" s="2">
         <v>7000</v>
@@ -7991,10 +7991,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>2293</v>
+        <v>2292</v>
       </c>
       <c r="D9" s="2">
         <v>8000</v>
@@ -8059,10 +8059,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>2294</v>
+        <v>2293</v>
       </c>
       <c r="D10" s="2">
         <v>9000</v>
@@ -8127,10 +8127,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="D11" s="2">
         <v>10000</v>
@@ -8195,10 +8195,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>2307</v>
+        <v>2306</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="D12" s="2">
         <v>11000</v>

</xml_diff>

<commit_message>
added threading for twitter fetches
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hadi\Desktop\kiki_crypto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1397E06-DD7C-4D3B-AE11-8BF40CCDF1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5D778A-9995-4971-AC24-970D73425504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12419" uniqueCount="2308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12421" uniqueCount="2310">
   <si>
     <t>UserNum</t>
   </si>
@@ -6949,6 +6949,12 @@
   </si>
   <si>
     <t>https://x.com/ordinalHO?t=jkhlbh&amp;s=04</t>
+  </si>
+  <si>
+    <t>Twitter_profile</t>
+  </si>
+  <si>
+    <t>Twitter_tweet</t>
   </si>
 </sst>
 </file>
@@ -7420,10 +7426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V1129"/>
+  <dimension ref="A1:X1129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7442,7 +7448,7 @@
     <col min="22" max="22" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7509,8 +7515,14 @@
       <c r="V1" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W1" s="7" t="s">
+        <v>2308</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -7578,7 +7590,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -7646,7 +7658,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -7714,7 +7726,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -7782,7 +7794,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -7850,7 +7862,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -7918,7 +7930,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -7986,7 +7998,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -8054,7 +8066,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -8122,7 +8134,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -8190,7 +8202,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -8258,7 +8270,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -8326,7 +8338,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -8394,7 +8406,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -8462,7 +8474,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
changed from printing response.content to response.text
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hadi\Desktop\kiki_crypto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B99BD05-B3FF-4FBB-87D1-D0642F9FE0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2589DE-55EC-415F-89F9-529A47A81606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7365,8 +7365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X1129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -84096,11 +84096,11 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{790F3371-4ED0-4ADB-AC8A-066D592A8DB9}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{105ED31F-5324-4C29-B25F-544CDE944917}"/>
-    <hyperlink ref="K3" r:id="rId3" xr:uid="{53B91BB7-022D-4EA2-82FB-C6B5995E7C1D}"/>
-    <hyperlink ref="Q2" r:id="rId4" xr:uid="{4E494935-AE25-4318-9626-B9CA2D001867}"/>
-    <hyperlink ref="Q3:Q1128" r:id="rId5" display="https://twitter.com/itstrahuna/status/1723186496985874758?t=QzeAE9GPVUoOZpx3uydvdg&amp;s=08" xr:uid="{86E62632-9240-417C-BF5C-9604C35EDC43}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{105ED31F-5324-4C29-B25F-544CDE944917}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{53B91BB7-022D-4EA2-82FB-C6B5995E7C1D}"/>
+    <hyperlink ref="Q2" r:id="rId3" xr:uid="{4E494935-AE25-4318-9626-B9CA2D001867}"/>
+    <hyperlink ref="Q3:Q1128" r:id="rId4" display="https://twitter.com/itstrahuna/status/1723186496985874758?t=QzeAE9GPVUoOZpx3uydvdg&amp;s=08" xr:uid="{86E62632-9240-417C-BF5C-9604C35EDC43}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{790F3371-4ED0-4ADB-AC8A-066D592A8DB9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>